<commit_message>
python version of PSI calculation - jupyter notebook first draft
</commit_message>
<xml_diff>
--- a/Turchin_Korotayev_R/PSImodel2020.xlsx
+++ b/Turchin_Korotayev_R/PSImodel2020.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F398A1F-19A4-409A-94A2-C4C31D98FF41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{5F398A1F-19A4-409A-94A2-C4C31D98FF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A795424-8728-4E1D-B734-A5AF1E13F142}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="1330" windowWidth="20080" windowHeight="12640" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="21" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="13">
   <si>
     <t>year</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>GDPpc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Distrust</t>
   </si>
   <si>
     <t>UnskillWage</t>
@@ -481,20 +478,20 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6328125" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" customWidth="1"/>
-    <col min="9" max="9" width="9.54296875" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -502,7 +499,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -514,16 +511,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>1</v>
@@ -532,7 +529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1945</v>
       </c>
@@ -560,7 +557,7 @@
       </c>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1946</v>
       </c>
@@ -588,7 +585,7 @@
       </c>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1947</v>
       </c>
@@ -616,7 +613,7 @@
       </c>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1948</v>
       </c>
@@ -644,7 +641,7 @@
       </c>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1949</v>
       </c>
@@ -672,7 +669,7 @@
       </c>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1950</v>
       </c>
@@ -700,7 +697,7 @@
       </c>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1951</v>
       </c>
@@ -728,7 +725,7 @@
       </c>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1952</v>
       </c>
@@ -756,7 +753,7 @@
       </c>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1953</v>
       </c>
@@ -784,7 +781,7 @@
       </c>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1954</v>
       </c>
@@ -812,7 +809,7 @@
       </c>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1955</v>
       </c>
@@ -840,7 +837,7 @@
       </c>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1956</v>
       </c>
@@ -864,11 +861,11 @@
         <v>13.225594512865786</v>
       </c>
       <c r="H13" s="4">
-        <v>63.243604938271609</v>
+        <v>63.243604938271602</v>
       </c>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1957</v>
       </c>
@@ -896,7 +893,7 @@
       </c>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1958</v>
       </c>
@@ -926,7 +923,7 @@
         <v>28.861406900000006</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1959</v>
       </c>
@@ -956,7 +953,7 @@
         <v>29.429347739999997</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1960</v>
       </c>
@@ -986,7 +983,7 @@
         <v>30.053954270000006</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1961</v>
       </c>
@@ -1016,7 +1013,7 @@
         <v>30.68988865</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1962</v>
       </c>
@@ -1046,7 +1043,7 @@
         <v>31.288487900000007</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1963</v>
       </c>
@@ -1076,7 +1073,7 @@
         <v>31.811734979999997</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1964</v>
       </c>
@@ -1106,7 +1103,7 @@
         <v>32.240326080000003</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1965</v>
       </c>
@@ -1136,7 +1133,7 @@
         <v>32.573076529999994</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1966</v>
       </c>
@@ -1166,7 +1163,7 @@
         <v>34.849735679999995</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1967</v>
       </c>
@@ -1196,7 +1193,7 @@
         <v>37.232026060000003</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1968</v>
       </c>
@@ -1226,7 +1223,7 @@
         <v>39.536229939999998</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1969</v>
       </c>
@@ -1256,7 +1253,7 @@
         <v>41.601396440000002</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1970</v>
       </c>
@@ -1286,7 +1283,7 @@
         <v>44.099466640000003</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1971</v>
       </c>
@@ -1316,7 +1313,7 @@
         <v>46.995730170000002</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1972</v>
       </c>
@@ -1346,7 +1343,7 @@
         <v>50.11854134</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1973</v>
       </c>
@@ -1376,7 +1373,7 @@
         <v>53.232805810000002</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1974</v>
       </c>
@@ -1406,7 +1403,7 @@
         <v>56.105944729999997</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1975</v>
       </c>
@@ -1436,7 +1433,7 @@
         <v>58.572409049999997</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1976</v>
       </c>
@@ -1466,7 +1463,7 @@
         <v>59.829563739999998</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1977</v>
       </c>
@@ -1496,7 +1493,7 @@
         <v>61.221275220000003</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1978</v>
       </c>
@@ -1526,7 +1523,7 @@
         <v>62.648147270000003</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1979</v>
       </c>
@@ -1556,7 +1553,7 @@
         <v>64.000489149999993</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1980</v>
       </c>
@@ -1586,7 +1583,7 @@
         <v>65.190008980000002</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1981</v>
       </c>
@@ -1616,7 +1613,7 @@
         <v>64.768043159999991</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1982</v>
       </c>
@@ -1646,7 +1643,7 @@
         <v>64.296849269999996</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1983</v>
       </c>
@@ -1676,7 +1673,7 @@
         <v>63.809257899999999</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1984</v>
       </c>
@@ -1706,7 +1703,7 @@
         <v>63.34287801</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1985</v>
       </c>
@@ -1736,7 +1733,7 @@
         <v>62.9291804</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1986</v>
       </c>
@@ -1766,7 +1763,7 @@
         <v>63.380818560000002</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1987</v>
       </c>
@@ -1796,7 +1793,7 @@
         <v>63.886711810000001</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1988</v>
       </c>
@@ -1826,7 +1823,7 @@
         <v>64.411957260000008</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1989</v>
       </c>
@@ -1856,7 +1853,7 @@
         <v>64.916024239999999</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1990</v>
       </c>
@@ -1886,7 +1883,7 @@
         <v>65.364525810000004</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1991</v>
       </c>
@@ -1916,7 +1913,7 @@
         <v>66.620891169999993</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1992</v>
       </c>
@@ -1946,7 +1943,7 @@
         <v>68.029911269999999</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1993</v>
       </c>
@@ -1976,7 +1973,7 @@
         <v>69.494767260000003</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1994</v>
       </c>
@@ -2006,7 +2003,7 @@
         <v>70.902416799999997</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1995</v>
       </c>
@@ -2036,7 +2033,7 @@
         <v>72.156428259999998</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1996</v>
       </c>
@@ -2066,7 +2063,7 @@
         <v>71.787802290000002</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1997</v>
       </c>
@@ -2096,7 +2093,7 @@
         <v>71.374084179999997</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1998</v>
       </c>
@@ -2126,7 +2123,7 @@
         <v>70.943632309999998</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1999</v>
       </c>
@@ -2156,7 +2153,7 @@
         <v>70.529664550000007</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>2000</v>
       </c>
@@ -2186,7 +2183,7 @@
         <v>70.160609840000006</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2001</v>
       </c>
@@ -2216,7 +2213,7 @@
         <v>70.298691820000002</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>2002</v>
       </c>
@@ -2246,7 +2243,7 @@
         <v>70.453825260000002</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2003</v>
       </c>
@@ -2276,7 +2273,7 @@
         <v>70.615413990000008</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>2004</v>
       </c>
@@ -2306,7 +2303,7 @@
         <v>70.770988700000004</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2005</v>
       </c>
@@ -2336,7 +2333,7 @@
         <v>70.909828540000007</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2006</v>
       </c>
@@ -2366,7 +2363,7 @@
         <v>71.528449469999998</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2007</v>
       </c>
@@ -2396,7 +2393,7 @@
         <v>72.225189239999992</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2008</v>
       </c>
@@ -2426,7 +2423,7 @@
         <v>72.952871399999992</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2009</v>
       </c>
@@ -2456,7 +2453,7 @@
         <v>73.655358339999992</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2010</v>
       </c>
@@ -2486,7 +2483,7 @@
         <v>74.283850119999997</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>2011</v>
       </c>
@@ -2516,7 +2513,7 @@
         <v>74.251934599999998</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2012</v>
       </c>
@@ -2539,7 +2536,7 @@
         <v>74.21574588</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2013</v>
       </c>
@@ -2551,7 +2548,7 @@
         <v>13.862754075527217</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>2014</v>
       </c>
@@ -2563,7 +2560,7 @@
         <v>13.816745032414177</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2015</v>
       </c>
@@ -2575,7 +2572,7 @@
         <v>13.74393434363277</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>2016</v>
       </c>
@@ -2587,7 +2584,7 @@
         <v>13.653187932703561</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>2017</v>
       </c>
@@ -2599,7 +2596,7 @@
         <v>13.545227294023549</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2018</v>
       </c>
@@ -2611,7 +2608,7 @@
         <v>13.415348452641886</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>2019</v>
       </c>
@@ -2623,7 +2620,7 @@
         <v>13.274121519625062</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2020</v>
       </c>
@@ -2646,23 +2643,23 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="6"/>
-    <col min="2" max="2" width="10.36328125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" style="6" customWidth="1"/>
-    <col min="4" max="5" width="8.7265625" style="6"/>
-    <col min="6" max="6" width="10.81640625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="10.6328125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="9.54296875" style="7" customWidth="1"/>
-    <col min="10" max="12" width="8.7265625" style="7"/>
+    <col min="1" max="1" width="8.77734375" style="6"/>
+    <col min="2" max="2" width="10.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="6" customWidth="1"/>
+    <col min="4" max="5" width="8.77734375" style="6"/>
+    <col min="6" max="6" width="10.77734375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="9.5546875" style="7" customWidth="1"/>
+    <col min="10" max="12" width="8.77734375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2670,7 +2667,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -2682,16 +2679,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>12</v>
-      </c>
       <c r="J1" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K1" s="9" t="s">
         <v>1</v>
@@ -2700,7 +2697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1945</v>
       </c>
@@ -2738,7 +2735,7 @@
         <v>7.5619583155688304</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1946</v>
       </c>
@@ -2776,7 +2773,7 @@
         <v>8.03875356477797</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1947</v>
       </c>
@@ -2814,7 +2811,7 @@
         <v>6.9715448046845303</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>1948</v>
       </c>
@@ -2852,7 +2849,7 @@
         <v>6.0761981213579004</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>1949</v>
       </c>
@@ -2890,7 +2887,7 @@
         <v>6.0856941660980901</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>1950</v>
       </c>
@@ -2928,7 +2925,7 @@
         <v>5.4162092893552201</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>1951</v>
       </c>
@@ -2966,7 +2963,7 @@
         <v>4.4478089345477301</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>1952</v>
       </c>
@@ -3004,7 +3001,7 @@
         <v>4.1437611175463402</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>1953</v>
       </c>
@@ -3042,7 +3039,7 @@
         <v>4.0178890239825602</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>1954</v>
       </c>
@@ -3080,7 +3077,7 @@
         <v>3.93940785844792</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>1955</v>
       </c>
@@ -3118,7 +3115,7 @@
         <v>3.43559369011858</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>1956</v>
       </c>
@@ -3156,7 +3153,7 @@
         <v>3.09510768093697</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>1957</v>
       </c>
@@ -3194,7 +3191,7 @@
         <v>2.7981950892070402</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>1958</v>
       </c>
@@ -3232,7 +3229,7 @@
         <v>2.7997920968835102</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>1959</v>
       </c>
@@ -3270,7 +3267,7 @@
         <v>2.5272576675098799</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>1960</v>
       </c>
@@ -3308,7 +3305,7 @@
         <v>2.3935901967077302</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>1961</v>
       </c>
@@ -3346,7 +3343,7 @@
         <v>2.3281184767263801</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>1962</v>
       </c>
@@ -3384,7 +3381,7 @@
         <v>2.1625493010343502</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>1963</v>
       </c>
@@ -3422,7 +3419,7 @@
         <v>2.0974574284491898</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>1964</v>
       </c>
@@ -3460,7 +3457,7 @@
         <v>1.9706022158618099</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>1965</v>
       </c>
@@ -3498,7 +3495,7 @@
         <v>1.8080099978068001</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>1966</v>
       </c>
@@ -3536,7 +3533,7 @@
         <v>1.7827802668744599</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>1967</v>
       </c>
@@ -3574,7 +3571,7 @@
         <v>1.9601728746322999</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>1968</v>
       </c>
@@ -3612,7 +3609,7 @@
         <v>2.0134144746884202</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>1969</v>
       </c>
@@ -3650,7 +3647,7 @@
         <v>2.05085443075727</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>1970</v>
       </c>
@@ -3688,7 +3685,7 @@
         <v>2.2223913156488799</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>1971</v>
       </c>
@@ -3726,7 +3723,7 @@
         <v>2.40716194440617</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>1972</v>
       </c>
@@ -3764,7 +3761,7 @@
         <v>2.4862364606610701</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>1973</v>
       </c>
@@ -3802,7 +3799,7 @@
         <v>2.4672824570230798</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>1974</v>
       </c>
@@ -3840,7 +3837,7 @@
         <v>2.5574972268246801</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>1975</v>
       </c>
@@ -3878,7 +3875,7 @@
         <v>2.9098875667980599</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>1976</v>
       </c>
@@ -3916,7 +3913,7 @@
         <v>3.0632367716037399</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>1977</v>
       </c>
@@ -3954,7 +3951,7 @@
         <v>3.0697586022396299</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>1978</v>
       </c>
@@ -3992,7 +3989,7 @@
         <v>3.0561316817993802</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>1979</v>
       </c>
@@ -4030,7 +4027,7 @@
         <v>3.02383163179866</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>1980</v>
       </c>
@@ -4068,7 +4065,7 @@
         <v>3.1667879147876601</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>1981</v>
       </c>
@@ -4106,7 +4103,7 @@
         <v>3.13458322121057</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
         <v>1982</v>
       </c>
@@ -4144,7 +4141,7 @@
         <v>3.5185802935103698</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
         <v>1983</v>
       </c>
@@ -4182,7 +4179,7 @@
         <v>3.7792482202441602</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
         <v>1984</v>
       </c>
@@ -4220,7 +4217,7 @@
         <v>4.0120173446192204</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
         <v>1985</v>
       </c>
@@ -4258,7 +4255,7 @@
         <v>4.4191889461030698</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
         <v>1986</v>
       </c>
@@ -4296,7 +4293,7 @@
         <v>4.6677674473311503</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>1987</v>
       </c>
@@ -4334,7 +4331,7 @@
         <v>4.99182849877515</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>1988</v>
       </c>
@@ -4372,7 +4369,7 @@
         <v>5.3100455459270099</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>1989</v>
       </c>
@@ -4410,7 +4407,7 @@
         <v>5.6669325556779597</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>1990</v>
       </c>
@@ -4448,7 +4445,7 @@
         <v>6.3542271881196903</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>1991</v>
       </c>
@@ -4486,7 +4483,7 @@
         <v>7.3703093536208302</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>1992</v>
       </c>
@@ -4524,7 +4521,7 @@
         <v>8.1329455115771694</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>1993</v>
       </c>
@@ -4562,7 +4559,7 @@
         <v>8.8426026376013294</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>1994</v>
       </c>
@@ -4600,7 +4597,7 @@
         <v>9.3696689165373304</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="6">
         <v>1995</v>
       </c>
@@ -4638,7 +4635,7 @@
         <v>10.11836799264</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="6">
         <v>1996</v>
       </c>
@@ -4676,7 +4673,7 @@
         <v>10.587406272092</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="6">
         <v>1997</v>
       </c>
@@ -4714,7 +4711,7 @@
         <v>10.870799466437701</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="6">
         <v>1998</v>
       </c>
@@ -4752,7 +4749,7 @@
         <v>11.1862405746829</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="6">
         <v>1999</v>
       </c>
@@ -4790,7 +4787,7 @@
         <v>11.4838406724788</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="6">
         <v>2000</v>
       </c>
@@ -4828,7 +4825,7 @@
         <v>11.5516453433863</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="6">
         <v>2001</v>
       </c>
@@ -4866,7 +4863,7 @@
         <v>12.2966319054973</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>2002</v>
       </c>
@@ -4904,7 +4901,7 @@
         <v>13.4967182379451</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="6">
         <v>2003</v>
       </c>
@@ -4942,7 +4939,7 @@
         <v>15.0188381491127</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>2004</v>
       </c>
@@ -4980,7 +4977,7 @@
         <v>16.5176922737772</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="6">
         <v>2005</v>
       </c>
@@ -5018,7 +5015,7 @@
         <v>18.134380296310599</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="6">
         <v>2006</v>
       </c>
@@ -5056,7 +5053,7 @@
         <v>20.147134615850199</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="6">
         <v>2007</v>
       </c>
@@ -5094,7 +5091,7 @@
         <v>22.298579906881201</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="6">
         <v>2008</v>
       </c>
@@ -5132,7 +5129,7 @@
         <v>25.932177771644799</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="6">
         <v>2009</v>
       </c>
@@ -5170,7 +5167,7 @@
         <v>33.062451061207703</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="6">
         <v>2010</v>
       </c>
@@ -5208,7 +5205,7 @@
         <v>40.075841270122702</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="6">
         <v>2011</v>
       </c>
@@ -5246,7 +5243,7 @@
         <v>44.8654623109704</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="6">
         <v>2012</v>
       </c>
@@ -5257,7 +5254,7 @@
         <v>17790</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E69" s="7">
         <v>0.68648036872495399</v>
@@ -5284,18 +5281,18 @@
         <v>49.957777562461999</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="6">
         <v>2013</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E70" s="7">
         <v>0.67579289594002201</v>
@@ -5322,18 +5319,18 @@
         <v>54.241408471793598</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="6">
         <v>2014</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E71" s="7">
         <v>0.66510542315509003</v>
@@ -5360,18 +5357,18 @@
         <v>58.982664627878599</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="6">
         <v>2015</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E72" s="7">
         <v>0.65441795037015804</v>
@@ -5398,18 +5395,18 @@
         <v>64.090702010436999</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="6">
         <v>2016</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E73" s="7">
         <v>0.64373047758522595</v>
@@ -5436,18 +5433,18 @@
         <v>69.629143545530795</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="6">
         <v>2017</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E74" s="7">
         <v>0.63304300480029296</v>
@@ -5474,18 +5471,18 @@
         <v>75.631868831740107</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="6">
         <v>2018</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E75" s="7">
         <v>0.62235553201536098</v>
@@ -5512,18 +5509,18 @@
         <v>82.101793345563607</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="6">
         <v>2019</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E76" s="7">
         <v>0.611668059230429</v>
@@ -5550,18 +5547,18 @@
         <v>89.133847511556993</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="6">
         <v>2020</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E77" s="7">
         <v>0.60098058644549701</v>
@@ -5588,52 +5585,52 @@
         <v>96.669817633433496</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C78" s="10"/>
       <c r="D78" s="11"/>
       <c r="E78" s="7"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C79" s="10"/>
       <c r="D79" s="11"/>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C80" s="10"/>
       <c r="D80" s="11"/>
       <c r="E80" s="7"/>
     </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C81" s="10"/>
       <c r="D81" s="11"/>
       <c r="E81" s="7"/>
     </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C82" s="10"/>
       <c r="D82" s="11"/>
       <c r="E82" s="7"/>
     </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C83" s="10"/>
       <c r="D83" s="11"/>
       <c r="E83" s="7"/>
     </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C84" s="10"/>
       <c r="D84" s="11"/>
       <c r="E84" s="7"/>
     </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C85" s="10"/>
       <c r="D85" s="11"/>
       <c r="E85" s="7"/>
     </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C86" s="10"/>
       <c r="D86" s="11"/>
       <c r="E86" s="7"/>
     </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C87" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Australian Political Stress indicator notebook
</commit_message>
<xml_diff>
--- a/Turchin_Korotayev_R/PSImodel2020.xlsx
+++ b/Turchin_Korotayev_R/PSImodel2020.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{5F398A1F-19A4-409A-94A2-C4C31D98FF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72279663-D9DB-4461-843D-BE02468F072A}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{5F398A1F-19A4-409A-94A2-C4C31D98FF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A0EF9EA-35BA-495E-9639-E793AC1941DE}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -477,8 +477,8 @@
   <dimension ref="A1:L77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K65" sqref="K65"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2643,7 +2643,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomLeft" sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>